<commit_message>
M2 - Stap 2: normalisering_v1 OK
</commit_message>
<xml_diff>
--- a/D2_NORMALISATIE/Recording Studios - Overzichtsdocument_v1.xlsx
+++ b/D2_NORMALISATIE/Recording Studios - Overzichtsdocument_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiv/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiv/Documents/GIT_DB2/matthias.vermeiren/D2_NORMALISATIE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E3F0636-CEC0-F249-9368-AAD32C3B8DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8810C859-DC76-C240-9BDA-4DE60896E8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58400" yWindow="-7300" windowWidth="26400" windowHeight="28300" xr2:uid="{32BA6673-E58A-2B48-8D43-D457B99DBC5E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{32BA6673-E58A-2B48-8D43-D457B99DBC5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>artist_id</t>
   </si>
@@ -153,9 +153,6 @@
     <t>singer</t>
   </si>
   <si>
-    <t>weekendje@gmail.com</t>
-  </si>
-  <si>
     <t>AR01</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Dynaudio</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>ProTools</t>
   </si>
   <si>
@@ -196,6 +190,18 @@
   </si>
   <si>
     <t>Redundantie-gevaar bij equipment! -&gt; to check</t>
+  </si>
+  <si>
+    <t>LA-2A compressor, 1176 compressor, Pultec</t>
+  </si>
+  <si>
+    <t>Melodyne, Fabfilter Bundle, iZotope Bundle</t>
+  </si>
+  <si>
+    <t>Moog, Roland, Nord Lead</t>
+  </si>
+  <si>
+    <t>theweeknd@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -279,6 +285,9 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -288,9 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -609,7 +615,7 @@
   <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,58 +629,61 @@
     <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="1" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="1" t="s">
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="1" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="3"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="6"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -805,112 +814,112 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="4">
-        <v>32854</v>
+      <c r="E3" s="1">
+        <v>32920</v>
       </c>
       <c r="F3">
         <v>478031245</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
         <v>39</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>40</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>41</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>42</v>
-      </c>
-      <c r="K3" t="s">
-        <v>43</v>
       </c>
       <c r="L3">
         <v>475021343</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
         <v>45</v>
       </c>
-      <c r="N3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>46</v>
       </c>
-      <c r="P3" t="s">
-        <v>47</v>
-      </c>
       <c r="Q3">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="R3">
         <v>100</v>
       </c>
       <c r="S3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V3">
         <v>90001</v>
       </c>
       <c r="W3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" t="s">
         <v>48</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z3" t="s">
         <v>49</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC3" t="s">
         <v>50</v>
       </c>
-      <c r="Z3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>52</v>
-      </c>
       <c r="AD3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AF3">
         <v>230315001</v>
       </c>
-      <c r="AG3" s="4">
+      <c r="AG3" s="1">
         <v>45000</v>
       </c>
-      <c r="AH3" s="6">
+      <c r="AH3" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="AI3" s="6">
+      <c r="AI3" s="3">
         <v>0.5</v>
       </c>
       <c r="AJ3">
         <v>1001</v>
       </c>
       <c r="AK3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AL3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
M2 - alles OK
</commit_message>
<xml_diff>
--- a/D2_NORMALISATIE/Recording Studios - Overzichtsdocument_v1.xlsx
+++ b/D2_NORMALISATIE/Recording Studios - Overzichtsdocument_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiv/Documents/GIT_DB2/matthias.vermeiren/D2_NORMALISATIE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8810C859-DC76-C240-9BDA-4DE60896E8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06E9EF7-FBA9-6E4B-93D8-6A42F4D45B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{32BA6673-E58A-2B48-8D43-D457B99DBC5E}"/>
+    <workbookView xWindow="33600" yWindow="-7800" windowWidth="51200" windowHeight="28800" xr2:uid="{32BA6673-E58A-2B48-8D43-D457B99DBC5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>artist_id</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Neumann</t>
-  </si>
-  <si>
-    <t>Redundantie-gevaar bij equipment! -&gt; to check</t>
   </si>
   <si>
     <t>LA-2A compressor, 1176 compressor, Pultec</t>
@@ -612,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49431F37-1F86-3D4E-99B6-1E386B361507}">
-  <dimension ref="A1:AL5"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,7 +818,7 @@
         <v>478031245</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
         <v>39</v>
@@ -875,16 +872,16 @@
         <v>48</v>
       </c>
       <c r="Y3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z3" t="s">
         <v>49</v>
       </c>
       <c r="AA3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB3" t="s">
         <v>53</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>54</v>
       </c>
       <c r="AC3" t="s">
         <v>50</v>
@@ -915,11 +912,6 @@
       </c>
       <c r="AL3" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>